<commit_message>
updated sean's bill of materials, ppt
</commit_message>
<xml_diff>
--- a/BillOfMaterials/Updated Bill of materials.xlsx
+++ b/BillOfMaterials/Updated Bill of materials.xlsx
@@ -39,46 +39,46 @@
     <t>Natural ABS 3mm Filament</t>
   </si>
   <si>
-    <t>Servo Motor</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10 piece rotarty encoder set</t>
-  </si>
-  <si>
-    <t>1/4th inch stainless steel screws</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/Stainless-Machine-Finish-Phillips-Threads/dp/B00DD49E98/ref=sr_1_3?s=industrial&amp;ie=UTF8&amp;qid=1379900567&amp;sr=1-3</t>
   </si>
   <si>
-    <t>5/16" rubber bands</t>
-  </si>
-  <si>
     <t>http://www.ebay.com/itm/1-Bag-Dental-Orthodontic-Rubber-Elastics-bands-5000pcs-bag-Force-4-5-OZ-5-16-/151127619288</t>
   </si>
   <si>
-    <t>Small Ball Bearings</t>
-  </si>
-  <si>
     <t>http://www.ebay.com/bhp/small-ball-bearings</t>
   </si>
   <si>
     <t>Total Price</t>
   </si>
   <si>
-    <t>VEX Robotics NiMH Robot Battery</t>
-  </si>
-  <si>
-    <t>Air Pincette Vacuum Tweezers</t>
-  </si>
-  <si>
-    <t>6' Silicone Air Line Tubing</t>
-  </si>
-  <si>
-    <t>1 pint Platex Mold Latex</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Detailed Plastic Acrylic based </t>
+    <t>30 bag 5/16" rubber bands</t>
+  </si>
+  <si>
+    <t>25 1/4th inch stainless steel screws</t>
+  </si>
+  <si>
+    <t>10 piece rotary encoder set</t>
+  </si>
+  <si>
+    <t>Servo motor</t>
+  </si>
+  <si>
+    <t>30 pack small ball bearings</t>
+  </si>
+  <si>
+    <t>VEX robotics NiMH robot battery</t>
+  </si>
+  <si>
+    <t>6' silicone air line tubing</t>
+  </si>
+  <si>
+    <t>1 pint Platex mold latex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detailed plastic acrylic based </t>
+  </si>
+  <si>
+    <t>Air Pincette vacuum tweezers</t>
   </si>
 </sst>
 </file>
@@ -89,7 +89,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,21 +104,70 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -129,11 +178,23 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -438,236 +499,241 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
         <v>75</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="6">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
         <v>74.989999999999995</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="6">
         <v>74.989999999999995</v>
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
         <v>37.950000000000003</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6">
         <v>37.950000000000003</v>
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
+    <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
         <v>10</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4">
         <v>7</v>
       </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>8.9499999999999993</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <v>62.65</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>25</v>
-      </c>
-      <c r="D8">
+    <row r="8" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
         <v>6.49</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="6">
         <v>6.49</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>30</v>
-      </c>
-      <c r="D9">
+    <row r="9" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
         <v>14.95</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6">
         <v>14.95</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
-        <v>30</v>
-      </c>
-      <c r="D10">
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
         <v>4.25</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="6">
         <v>4.95</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
         <v>19.989999999999998</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="6">
         <v>19.989999999999998</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="12" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3.33</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>3.33</v>
-      </c>
-      <c r="E12" s="1">
-        <v>3.33</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5">
+        <v>36</v>
+      </c>
+      <c r="E13" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>36</v>
-      </c>
-      <c r="E13" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2.99</v>
+      </c>
+      <c r="E14" s="6">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>2.99</v>
-      </c>
-      <c r="E14" s="1">
-        <v>32.4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
         <v>75</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="6">
         <v>75</v>
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1">
+    <row r="16" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="8">
         <f>SUM(E3:E15)</f>
         <v>453.69999999999993</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>